<commit_message>
Fixed getstartparams test in selendroid
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/System_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/System_JS.xlsx
@@ -180,18 +180,6 @@
 validate4;</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(system_test_link);
-validate2;
-SelectTestToRun(VT200_0963_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;
-</t>
-  </si>
-  <si>
     <t>wait(3);
 validate1;
 link_Click(system_test_link);
@@ -434,24 +422,6 @@
 validate4
 {
 validate_SystemProperties=getallproperties
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=System JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0963
-};
-validate4
-{
-validate_Result=?
 };</t>
   </si>
   <si>
@@ -595,6 +565,48 @@
 validate4;
 CheckUITextContains(https://www.google.co.in);
 press_Key(Back);</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(system_test_link);
+validate2;
+SelectTestToRun(VT200_0963_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+SelectTestToRun(VT200_0959_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
+TaponGetStartparams;
+validate5;
+CheckUITextContains(?ParamsAreSet);
+ClickUIButtonText(OK);
+press_Key(Back);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=System JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0963
+};
+validate4
+{
+validate_Text_Exists=VT200-0959
+};
+validate5
+{
+validate_App_Launched_Device=com.rhomobile.testapp
+};</t>
   </si>
 </sst>
 </file>
@@ -1074,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1133,7 +1145,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>19</v>
@@ -1142,10 +1154,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>10</v>
@@ -1162,7 +1174,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>20</v>
@@ -1171,10 +1183,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="2"/>
@@ -1189,7 +1201,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>21</v>
@@ -1201,7 +1213,7 @@
         <v>30</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="2"/>
@@ -1216,7 +1228,7 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>11</v>
@@ -1225,10 +1237,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -1243,7 +1255,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>12</v>
@@ -1270,7 +1282,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>13</v>
@@ -1279,16 +1291,16 @@
         <v>1</v>
       </c>
       <c r="G7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="255.75" thickBot="1">
+    <row r="8" spans="1:11" ht="268.5" thickBot="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1297,25 +1309,25 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F8" s="9">
         <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="217.5" thickBot="1">
+    <row r="9" spans="1:11" ht="255.75" thickBot="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1324,25 +1336,25 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="9">
         <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="204.75" thickBot="1">
+    <row r="10" spans="1:11" ht="217.5" thickBot="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1351,19 +1363,19 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -1378,19 +1390,19 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F11" s="9">
         <v>1</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -1405,7 +1417,7 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>25</v>
@@ -1414,10 +1426,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -1432,7 +1444,7 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>26</v>
@@ -1441,10 +1453,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -1459,7 +1471,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>27</v>
@@ -1468,10 +1480,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -1486,7 +1498,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>28</v>
@@ -1495,10 +1507,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -1513,7 +1525,7 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>29</v>
@@ -1522,10 +1534,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -1540,7 +1552,7 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>17</v>
@@ -1549,10 +1561,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>

</xml_diff>